<commit_message>
run all _ v1: conversation id: 17485 17486 17487 17488 17489 (của bài 321) - rull All 5 cái: work
</commit_message>
<xml_diff>
--- a/7_eval_compareFastResponse/eval/conversation_17485_output_eval.xlsx
+++ b/7_eval_compareFastResponse/eval/conversation_17485_output_eval.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,57 +458,71 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>[{"role": "assistant", "content": "Chào cậu! Bữa nay thầy giáo robot trên sao HỎA dạy tớ cách luyện nói theo nhịp như… hát rap đó! Mỗi cụm từ giống như một đoạn nhạc nhỏ, có nhịp điệu riêng."}]</t>
+          <t>[{"role": "assistant", "content": "Chào cậu! Bữa nay thầy giáo robot trên sao HỎA dạy tớ cách luyện nói theo nhịp như… hát rap đó! Mỗi cụm từ giống như một đoạn nhạc nhỏ, có nhịp điệu riêng."}, {"role": "assistant", "content": "Cứ theo nhịp là nói được tiếng Anh hay hơn liền! Giờ tụi mình thử cùng luyện nha. Cậu đã sẵn sàng chưa?"}, {"role": "user", "content": "[NEXT]"}]</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Cứ theo nhịp là nói được tiếng Anh hay hơn liền! Giờ tụi mình thử cùng luyện nha. Cậu đã sẵn sàng chưa?</t>
+          <t>Chào cậu! Bữa nay thầy giáo robot trên sao HỎA dạy tớ cách luyện nói theo nhịp như… hát rap đó! Mỗi cụm từ giống như một đoạn nhạc nhỏ, có nhịp điệu riêng.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Tuyệt! Nhịp điệu nào cũng hay như ca khúc mới! 🎤</t>
+          <t>Okay, let's see. The user just said "NEXT" after a previous message where they were talking about learning to speak English with a teacher robot. The assistant responded with an encouraging message about following the rhythm and asking if the user is ready. Now the user has written "NEXT". 
+First, I need to figure out the emotion in the latest message. The word "NEXT" is pretty neutral, but in the context of learning and practice, it might indicate a positive move forward. The user might be excited or motivated to continue the activity.
+The previous interaction was about learning English through a teacher robot, using a rap-like approach. The assistant encouraged the user to keep going and asked if they were ready. Now, the user's response is "NEXT", which could be a signal to move on to the next step in the activity.
+Since the user is continuing the practice, the emotion here is likely positive, possibly excited or determined. The assistant needs to respond in a friendly, informal way that mirrors this positive emotion. The response should be short, 1-8 words, and in English or Vietnamese. The user's previous messages were in Vietnamese, but the assistant's response was in English. However, the user might be comfortable with either language. 
+The instruction says to reply in the same language as the latest message. The latest message is "NEXT", which is in English. However, the previous messages were in Vietnamese. But the user might be switching back to English. Alternatively, the user might not care about the language and just want a quick response.
+The assistant's task is to detect the emotion in the latest message and reply in the same language. Since "NEXT" is a neutral word, but in the context of learning, it's positive. The assistant should respond with something encouraging, maybe using an emoji or an exclamation mark to show enthusiasm. 
+Possible responses could be "Next up! 🎤!" or "Let's go! 🚀!" in English, or "Tiếp theo! 🎤" in Vietnamese. However, the user's previous message was in Vietnamese, so maybe they are continuing in Vietnamese. But the assistant's previous response was in English, so it's a bit confusing.
+But the user's latest message is "NEXT" which is in English. However, the user might be using "NEXT" as a command to continue the activity. The assistant should respond in English, as that's the language of the latest message. The response should be short, friendly, and positive. 
+So, the best response would be something like "Next up! 🎤!" or "Let's go! 🚀!" to keep the energy high and encourage the user to continue. Using an emoji adds a friendly touch. The response should be under 60 characters, so "Next up! 🎤!" is 10 characters, which is well within the limit.
+&lt;/think&gt;
+Next up! 🎤</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>[{"role": "assistant", "content": "Cứ theo nhịp là nói được tiếng Anh hay hơn liền! Giờ tụi mình thử cùng luyện nha. Cậu đã sẵn sàng chưa?"}, {"role": "user", "content": "[NEXT]"}]</t>
+          <t>[{"role": "assistant", "content": "Chào cậu! Bữa nay thầy giáo robot trên sao HỎA dạy tớ cách luyện nói theo nhịp như… hát rap đó! Mỗi cụm từ giống như một đoạn nhạc nhỏ, có nhịp điệu riêng."}, {"role": "assistant", "content": "Cứ theo nhịp là nói được tiếng Anh hay hơn liền! Giờ tụi mình thử cùng luyện nha. Cậu đã sẵn sàng chưa?"}, {"role": "user", "content": "[NEXT]"}, {"role": "assistant", "content": "Yên tâm nha! Cậu không học một mình đâu, Pika luôn bên cạnh nè! chúng mình sẽ học nói tiếng Anh theo nhịp giống như hát nha! Bài hát này có nhiều cụm từ rất quen mà cũng rất vui. Bài đầu tiên nha. Đầu tiên, cậu hãy nghe thử cả bài nhé, đừng hát theo vội. Mình chỉ cần cảm nhịp thôi."}, {"role": "assistant", "content": "Giờ mình cùng lặp lại đoạn đầu tiên nha, câu chào cực kỳ thân thiện luôn nè."}, {"role": "assistant", "content": "Cậu nói lại cùng tớ nha."}, {"role": "user", "content": "Hello, hello, hello, how are you? Hello, hello, hello, how are you?"}]</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Yên tâm nha! Cậu không học một mình đâu, Pika luôn bên cạnh nè! chúng mình sẽ học nói tiếng Anh theo nhịp giống như hát nha! Bài hát này có nhiều cụm từ rất quen mà cũng rất vui. Bài đầu tiên nha. Đầu tiên, cậu hãy nghe thử cả bài nhé, đừng hát theo vội. Mình chỉ cần cảm nhịp thôi. </t>
+          <t>Cứ theo nhịp là nói được tiếng Anh hay hơn liền! Giờ tụi mình thử cùng luyện nha. Cậu đã sẵn sàng chưa?</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Okay, let's go! Ready to chat? 😊</t>
+          <t>Tuyệt! Cậu đã nói được rồi! Cảm ơn cậu đã luyện tập nhé!</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>[{"role": "assistant", "content": "Yên tâm nha! Cậu không học một mình đâu, Pika luôn bên cạnh nè! chúng mình sẽ học nói tiếng Anh theo nhịp giống như hát nha! Bài hát này có nhiều cụm từ rất quen mà cũng rất vui. Bài đầu tiên nha. Đầu tiên, cậu hãy nghe thử cả bài nhé, đừng hát theo vội. Mình chỉ cần cảm nhịp thôi. "}]</t>
+          <t>[{"role": "assistant", "content": "Chào cậu! Bữa nay thầy giáo robot trên sao HỎA dạy tớ cách luyện nói theo nhịp như… hát rap đó! Mỗi cụm từ giống như một đoạn nhạc nhỏ, có nhịp điệu riêng."}, {"role": "assistant", "content": "Cứ theo nhịp là nói được tiếng Anh hay hơn liền! Giờ tụi mình thử cùng luyện nha. Cậu đã sẵn sàng chưa?"}, {"role": "user", "content": "[NEXT]"}, {"role": "assistant", "content": "Yên tâm nha! Cậu không học một mình đâu, Pika luôn bên cạnh nè! chúng mình sẽ học nói tiếng Anh theo nhịp giống như hát nha! Bài hát này có nhiều cụm từ rất quen mà cũng rất vui. Bài đầu tiên nha. Đầu tiên, cậu hãy nghe thử cả bài nhé, đừng hát theo vội. Mình chỉ cần cảm nhịp thôi."}, {"role": "assistant", "content": "Giờ mình cùng lặp lại đoạn đầu tiên nha, câu chào cực kỳ thân thiện luôn nè."}, {"role": "assistant", "content": "Cậu nói lại cùng tớ nha."}, {"role": "user", "content": "Hello, hello, hello, how are you? Hello, hello, hello, how are you?"}, {"role": "assistant", "content": "Nice! You did it! Tiếp theo là khi mình cảm thấy thật tuyệt, cùng nói theo nhịp nha!"}, {"role": "assistant", "content": "Nào, nói lại với tớ!"}, {"role": "user", "content": "I'm good. I'm rich. I'm wonderful."}]</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Yên tâm nha! Cậu không học một mình đâu, Pika luôn bên cạnh nè! chúng mình sẽ học nói tiếng Anh theo nhịp giống như hát nha! Bài hát này có nhiều cụm từ rất quen mà cũng rất vui. Bài đầu tiên nha. Đầu tiên, cậu hãy nghe thử cả bài nhé, đừng hát theo vội. Mình chỉ cần cảm nhịp thôi. </t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Okay, let's see. The user is talking about learning English with a song, specifically mentioning "Pika" and a song that's fun and has familiar phrases. They want to start with the first verse, listening first before singing along. The user seems to be encouraging and supportive, maybe a bit nervous but trying to stay positive. The response should be in Vietnamese, friendly, and short. Maybe something like "Chào mừng! Cảm ơn vì đã chia sẻ!" to acknowledge their participation and keep the mood positive. Keep it simple and encouraging.</t>
+          <t>Tuyệt quá! Mình yêu cách cậu nói!</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>[{"role": "assistant", "content": ""}]</t>
+          <t>[{"role": "assistant", "content": "Chào cậu! Bữa nay thầy giáo robot trên sao HỎA dạy tớ cách luyện nói theo nhịp như… hát rap đó! Mỗi cụm từ giống như một đoạn nhạc nhỏ, có nhịp điệu riêng."}, {"role": "assistant", "content": "Cứ theo nhịp là nói được tiếng Anh hay hơn liền! Giờ tụi mình thử cùng luyện nha. Cậu đã sẵn sàng chưa?"}, {"role": "user", "content": "[NEXT]"}, {"role": "assistant", "content": "Yên tâm nha! Cậu không học một mình đâu, Pika luôn bên cạnh nè! chúng mình sẽ học nói tiếng Anh theo nhịp giống như hát nha! Bài hát này có nhiều cụm từ rất quen mà cũng rất vui. Bài đầu tiên nha. Đầu tiên, cậu hãy nghe thử cả bài nhé, đừng hát theo vội. Mình chỉ cần cảm nhịp thôi."}, {"role": "assistant", "content": "Giờ mình cùng lặp lại đoạn đầu tiên nha, câu chào cực kỳ thân thiện luôn nè."}, {"role": "assistant", "content": "Cậu nói lại cùng tớ nha."}, {"role": "user", "content": "Hello, hello, hello, how are you? Hello, hello, hello, how are you?"}, {"role": "assistant", "content": "Nice! You did it! Tiếp theo là khi mình cảm thấy thật tuyệt, cùng nói theo nhịp nha!"}, {"role": "assistant", "content": "Nào, nói lại với tớ!"}, {"role": "user", "content": "I'm good. I'm rich. I'm wonderful."}, {"role": "assistant", "content": "Awesome! Cậu nói theo nhịp rất tốt! Câu chào quen thuộc quay lại nè! Mình cùng nói lại một lần nữa nhé!"}, {"role": "assistant", "content": "Cậu nhớ nhịp rồi đúng không? Cùng nói nào!"}, {"role": "user", "content": "Hello! Hello!"}]</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -519,374 +533,61 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Okay, I'm here to help. What's on your mind?</t>
+          <t>Tốt lắm! Nhịp rất đẹp! Cậu thật sự làm được rồi!</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>[{"role": "assistant", "content": "Giờ mình cùng lặp lại đoạn đầu tiên nha, câu chào cực kỳ thân thiện luôn nè."}]</t>
+          <t>[{"role": "assistant", "content": "Chào cậu! Bữa nay thầy giáo robot trên sao HỎA dạy tớ cách luyện nói theo nhịp như… hát rap đó! Mỗi cụm từ giống như một đoạn nhạc nhỏ, có nhịp điệu riêng."}, {"role": "assistant", "content": "Cứ theo nhịp là nói được tiếng Anh hay hơn liền! Giờ tụi mình thử cùng luyện nha. Cậu đã sẵn sàng chưa?"}, {"role": "user", "content": "[NEXT]"}, {"role": "assistant", "content": "Yên tâm nha! Cậu không học một mình đâu, Pika luôn bên cạnh nè! chúng mình sẽ học nói tiếng Anh theo nhịp giống như hát nha! Bài hát này có nhiều cụm từ rất quen mà cũng rất vui. Bài đầu tiên nha. Đầu tiên, cậu hãy nghe thử cả bài nhé, đừng hát theo vội. Mình chỉ cần cảm nhịp thôi."}, {"role": "assistant", "content": "Giờ mình cùng lặp lại đoạn đầu tiên nha, câu chào cực kỳ thân thiện luôn nè."}, {"role": "assistant", "content": "Cậu nói lại cùng tớ nha."}, {"role": "user", "content": "Hello, hello, hello, how are you? Hello, hello, hello, how are you?"}, {"role": "assistant", "content": "Nice! You did it! Tiếp theo là khi mình cảm thấy thật tuyệt, cùng nói theo nhịp nha!"}, {"role": "assistant", "content": "Nào, nói lại với tớ!"}, {"role": "user", "content": "I'm good. I'm rich. I'm wonderful."}, {"role": "assistant", "content": "Awesome! Cậu nói theo nhịp rất tốt! Câu chào quen thuộc quay lại nè! Mình cùng nói lại một lần nữa nhé!"}, {"role": "assistant", "content": "Cậu nhớ nhịp rồi đúng không? Cùng nói nào!"}, {"role": "user", "content": "Hello! Hello!"}, {"role": "assistant", "content": "Good job! Cậu nhớ rất giỏi! Đôi khi mình cũng cảm thấy hơi mệt hoặc đói. Vậy thì mình sẽ nói thế này nè"}, {"role": "assistant", "content": "Giờ thì cậu nhại theo tớ nha!"}, {"role": "user", "content": "I'm tired I'm hungry I'm not so good I'm tired"}]</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Cậu nói lại cùng tớ nha.</t>
+        </is>
+      </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Chào bạn nhé! 😊</t>
+          <t>Tớ cũng thế! Cảm giác đó rất quen thuộc nè!</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>[{"role": "assistant", "content": ""}]</t>
+          <t>[{"role": "assistant", "content": "Chào cậu! Bữa nay thầy giáo robot trên sao HỎA dạy tớ cách luyện nói theo nhịp như… hát rap đó! Mỗi cụm từ giống như một đoạn nhạc nhỏ, có nhịp điệu riêng."}, {"role": "assistant", "content": "Cứ theo nhịp là nói được tiếng Anh hay hơn liền! Giờ tụi mình thử cùng luyện nha. Cậu đã sẵn sàng chưa?"}, {"role": "user", "content": "[NEXT]"}, {"role": "assistant", "content": "Yên tâm nha! Cậu không học một mình đâu, Pika luôn bên cạnh nè! chúng mình sẽ học nói tiếng Anh theo nhịp giống như hát nha! Bài hát này có nhiều cụm từ rất quen mà cũng rất vui. Bài đầu tiên nha. Đầu tiên, cậu hãy nghe thử cả bài nhé, đừng hát theo vội. Mình chỉ cần cảm nhịp thôi."}, {"role": "assistant", "content": "Giờ mình cùng lặp lại đoạn đầu tiên nha, câu chào cực kỳ thân thiện luôn nè."}, {"role": "assistant", "content": "Cậu nói lại cùng tớ nha."}, {"role": "user", "content": "Hello, hello, hello, how are you? Hello, hello, hello, how are you?"}, {"role": "assistant", "content": "Nice! You did it! Tiếp theo là khi mình cảm thấy thật tuyệt, cùng nói theo nhịp nha!"}, {"role": "assistant", "content": "Nào, nói lại với tớ!"}, {"role": "user", "content": "I'm good. I'm rich. I'm wonderful."}, {"role": "assistant", "content": "Awesome! Cậu nói theo nhịp rất tốt! Câu chào quen thuộc quay lại nè! Mình cùng nói lại một lần nữa nhé!"}, {"role": "assistant", "content": "Cậu nhớ nhịp rồi đúng không? Cùng nói nào!"}, {"role": "user", "content": "Hello! Hello!"}, {"role": "assistant", "content": "Good job! Cậu nhớ rất giỏi! Đôi khi mình cũng cảm thấy hơi mệt hoặc đói. Vậy thì mình sẽ nói thế này nè"}, {"role": "assistant", "content": "Giờ thì cậu nhại theo tớ nha!"}, {"role": "user", "content": "I'm tired I'm hungry I'm not so good I'm tired"}, {"role": "assistant", "content": "Great! Bây giờ mình cùng nói câu chào cuối nhé! Và cuối cùng, bài hát kết thúc bằng câu chào quen thuộc một lần nữa. Nói lại lần cuối nha!"}, {"role": "assistant", "content": "Cùng nói lại với tớ nào!"}, {"role": "user", "content": "Hello, hello, hello, how are you?"}]</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Cậu nói lại cùng tớ nha.</t>
+          <t xml:space="preserve">Nice! You did it! Tiếp theo là khi mình cảm thấy thật tuyệt, cùng nói theo nhịp nha! </t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Okay, I'll help you with that. Please share the message you want me to analyze.</t>
+          <t>Perfect! Cậu đã học rất tốt! Chúc mừng nhé!</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>[{"role": "assistant", "content": "Cậu nói lại cùng tớ nha."}, {"role": "user", "content": "Hello, hello, hello, how are you? Hello, hello, hello, how are you?"}]</t>
+          <t>[{"role": "assistant", "content": "Chào cậu! Bữa nay thầy giáo robot trên sao HỎA dạy tớ cách luyện nói theo nhịp như… hát rap đó! Mỗi cụm từ giống như một đoạn nhạc nhỏ, có nhịp điệu riêng."}, {"role": "assistant", "content": "Cứ theo nhịp là nói được tiếng Anh hay hơn liền! Giờ tụi mình thử cùng luyện nha. Cậu đã sẵn sàng chưa?"}, {"role": "user", "content": "[NEXT]"}, {"role": "assistant", "content": "Yên tâm nha! Cậu không học một mình đâu, Pika luôn bên cạnh nè! chúng mình sẽ học nói tiếng Anh theo nhịp giống như hát nha! Bài hát này có nhiều cụm từ rất quen mà cũng rất vui. Bài đầu tiên nha. Đầu tiên, cậu hãy nghe thử cả bài nhé, đừng hát theo vội. Mình chỉ cần cảm nhịp thôi."}, {"role": "assistant", "content": "Giờ mình cùng lặp lại đoạn đầu tiên nha, câu chào cực kỳ thân thiện luôn nè."}, {"role": "assistant", "content": "Cậu nói lại cùng tớ nha."}, {"role": "user", "content": "Hello, hello, hello, how are you? Hello, hello, hello, how are you?"}, {"role": "assistant", "content": "Nice! You did it! Tiếp theo là khi mình cảm thấy thật tuyệt, cùng nói theo nhịp nha!"}, {"role": "assistant", "content": "Nào, nói lại với tớ!"}, {"role": "user", "content": "I'm good. I'm rich. I'm wonderful."}, {"role": "assistant", "content": "Awesome! Cậu nói theo nhịp rất tốt! Câu chào quen thuộc quay lại nè! Mình cùng nói lại một lần nữa nhé!"}, {"role": "assistant", "content": "Cậu nhớ nhịp rồi đúng không? Cùng nói nào!"}, {"role": "user", "content": "Hello! Hello!"}, {"role": "assistant", "content": "Good job! Cậu nhớ rất giỏi! Đôi khi mình cũng cảm thấy hơi mệt hoặc đói. Vậy thì mình sẽ nói thế này nè"}, {"role": "assistant", "content": "Giờ thì cậu nhại theo tớ nha!"}, {"role": "user", "content": "I'm tired I'm hungry I'm not so good I'm tired"}, {"role": "assistant", "content": "Great! Bây giờ mình cùng nói câu chào cuối nhé! Và cuối cùng, bài hát kết thúc bằng câu chào quen thuộc một lần nữa. Nói lại lần cuối nha!"}, {"role": "assistant", "content": "Cùng nói lại với tớ nào!"}, {"role": "user", "content": "Hello, hello, hello, how are you?"}, {"role": "assistant", "content": "Well done! Giờ thì mình cùng hát lại từ đầu đến cuối bài hát này nhé, lần này cậu có thể vừa hát vừa nhún nhảy cho vui luôn nha!"}, {"role": "assistant", "content": "Tiếp theo, hãy tưởng tượng mình sẽ bắt đầu một ngày mới thật vui bằng một bài hát tiếng Anh siêu rộn ràng nha. Cậu sẽ được luyện các câu chào buổi sáng theo nhịp. Vừa học, vừa hát, vừa nhảy cũng được luôn! Cậu sẵn sàng chưa?"}, {"role": "user", "content": "I'm ready."}]</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nice! You did it! Tiếp theo là khi mình cảm thấy thật tuyệt, cùng nói theo nhịp nha! </t>
+          <t>Nào, nói lại với tớ!</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Hello again! How are you? 😊</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>[{"role": "assistant", "content": "Nice! You did it! Tiếp theo là khi mình cảm thấy thật tuyệt, cùng nói theo nhịp nha! "}]</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Mình đồng hành cùng bạn nhé! 🌟</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>[{"role": "assistant", "content": ""}]</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Nào, nói lại với tớ!</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Okay, I'm here to help. What's on your mind?</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>[{"role": "assistant", "content": "Nào, nói lại với tớ!"}, {"role": "user", "content": "I'm good. I'm rich. I'm wonderful."}]</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Awesome! Cậu nói theo nhịp rất tốt! Câu chào quen thuộc quay lại nè! Mình cùng nói lại một lần nữa nhé!</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>That's great to hear! 🎉</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>[{"role": "assistant", "content": "Awesome! Cậu nói theo nhịp rất tốt! Câu chào quen thuộc quay lại nè! Mình cùng nói lại một lần nữa nhé!"}]</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Chào lại! Cảm ơn cậu! 😊</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>[{"role": "assistant", "content": ""}]</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Cậu nhớ nhịp rồi đúng không? Cùng nói nào!</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Okay, I'm ready. Just send me the message and I'll respond instantly with the right emotion in the same language, keeping it short and friendly. Let me know when you're ready!</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>[{"role": "assistant", "content": "Cậu nhớ nhịp rồi đúng không? Cùng nói nào!"}, {"role": "user", "content": "Hello! Hello!"}]</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Good job! Cậu nhớ rất giỏi! Đôi khi mình cũng cảm thấy hơi mệt hoặc đói. Vậy thì mình sẽ nói thế này nè</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Hello again! 😊</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>[{"role": "assistant", "content": "Good job! Cậu nhớ rất giỏi! Đôi khi mình cũng cảm thấy hơi mệt hoặc đói. Vậy thì mình sẽ nói thế này nè"}]</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Mệt thì nghỉ ngơi, đói thì ăn cơm nhé! 😊</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>[{"role": "assistant", "content": ""}]</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Giờ thì cậu nhại theo tớ nha!</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Okay, I see. Let me try to figure this out. The user wants me to act as QuickReact, which means I need to detect the emotion in the latest message and respond in the same language, either English or Vietnamese. The response should be 1-8 words, up to 60 characters, and in a friendly, informal tone that mirrors the emotion. If the message is sad, I should soothe; if happy, cheer; if worried, reassure. Also, emojis or exclamation points are welcome. The output should only be that text, no explanations.
-First, I need to check the latest message. Wait, the user hasn't provided any specific message yet. The example given is a prompt for the assistant, not an actual message. So maybe the user is testing if I understand the process. But according to the instructions, I should only respond to the latest message. Since there's no message provided, maybe I should ask for clarification? But the user said to output only that text, so maybe I should respond with a placeholder or something. However, the example shows that when there's no message, the assistant might respond with a default. Wait, in the example, the user's message is "You are QuickReact..." and the assistant's response is "Okay, I see." So maybe in this case, since there's no actual message to process, the assistant just confirms understanding. But the user might be expecting the assistant to process a message. Since there's no message, perhaps the assistant should respond with a default like "Okay, I see." or something similar. But the user's instruction says to output only the text, so I should just provide that. So the answer would be "Okay, I see." but in the required language. Wait, the user might have a message in Vietnamese or English. But since the user's message is in English, the response should be in English. So the answer is "Okay, I see." but shorter. Wait, the example response is "Okay, I see." which is 4 words. That fits the criteria. So maybe the correct response is "Okay, I see." as per the example. But the user might be expecting something else. However, since there's no message, the assistant can't process it, so the example response is appropriate.
-&lt;/think&gt;
-Okay, I see.</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>[{"role": "assistant", "content": " Giờ thì cậu nhại theo tớ nha!"}, {"role": "user", "content": "I'm tired I'm hungry I'm not so good I'm tired"}]</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Great! Bây giờ mình cùng nói câu chào cuối nhé! Và cuối cùng, bài hát kết thúc bằng câu chào quen thuộc một lần nữa. Nói lại lần cuối nha! </t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>I'm here for you. Take your time.</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>[{"role": "assistant", "content": "Great! Bây giờ mình cùng nói câu chào cuối nhé! Và cuối cùng, bài hát kết thúc bằng câu chào quen thuộc một lần nữa. Nói lại lần cuối nha! "}]</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Chào buổi sáng! 😊</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>[{"role": "assistant", "content": ""}]</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Cùng nói lại với tớ nào!</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Okay, I'm ready. Just need to wait for the next message.</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>[{"role": "assistant", "content": "Cùng nói lại với tớ nào!"}, {"role": "user", "content": "Hello, hello, hello, how are you?"}]</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Well done! Giờ thì mình cùng hát lại từ đầu đến cuối bài hát này nhé, lần này cậu có thể vừa hát vừa nhún nhảy cho vui luôn nha! </t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Hihi, đang vui đây! 😄</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>[{"role": "assistant", "content": "Well done! Giờ thì mình cùng hát lại từ đầu đến cuối bài hát này nhé, lần này cậu có thể vừa hát vừa nhún nhảy cho vui luôn nha! "}]</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Chào cậu, mình đợi cậu hát nhé! 😊</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>[{"role": "assistant", "content": ""}]</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Tiếp theo, hãy tưởng tượng mình sẽ bắt đầu một ngày mới thật vui bằng một bài hát tiếng Anh siêu rộn ràng nha. Cậu sẽ được luyện các câu chào buổi sáng theo nhịp. Vừa học, vừa hát, vừa nhảy cũng được luôn! Cậu sẵn sàng chưa?</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Okay, I'll help you with that. Just send me the message you want me to analyze, and I'll detect the emotion and respond appropriately in the same language, keeping it short and friendly.</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>[{"role": "assistant", "content": "Tiếp theo, hãy tưởng tượng mình sẽ bắt đầu một ngày mới thật vui bằng một bài hát tiếng Anh siêu rộn ràng nha. Cậu sẽ được luyện các câu chào buổi sáng theo nhịp. Vừa học, vừa hát, vừa nhảy cũng được luôn! Cậu sẵn sàng chưa?"}, {"role": "user", "content": "I'm ready."}]</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Great! Let's start! Đầu tiên, mình nghe trọn bài hát để quen với nhịp, giai điệu và các cụm từ hay dùng vào buổi sáng nha! </t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Great! Let's sing and dance! 🎶💃</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>[{"role": "assistant", "content": "Great! Let's start! Đầu tiên, mình nghe trọn bài hát để quen với nhịp, giai điệu và các cụm từ hay dùng vào buổi sáng nha! "}]</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Nhạc dễ nghe, mình yêu! 🎶</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>[{"role": "assistant", "content": ""}]</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Mình bắt đầu với câu chào buổi sáng nha, thật tươi lên nào! </t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Okay, I'm here to help. What's on your mind?</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>[{"role": "assistant", "content": "Mình bắt đầu với câu chào buổi sáng nha, thật tươi lên nào! "}]</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>Chào buổi sáng! 🌞 Cảm thấy tốt không?</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>[{"role": "assistant", "content": ""}]</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Nào, lặp lại cùng tớ nhé!</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Okay, I'm ready. Just wait for the message.</t>
+          <t>Chúng mình bắt đầu ngay nhé!</t>
         </is>
       </c>
     </row>

</xml_diff>